<commit_message>
adding a design doc
Added file to display JSON Format
</commit_message>
<xml_diff>
--- a/MS-DB/DB api manual.xlsx
+++ b/MS-DB/DB api manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\MS-DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7EC179F-D110-4A29-910F-9A33C660289D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48224A2E-A19F-4C04-904B-C3DC62F15CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7107093B-2C12-4176-8665-F241E905E88A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>对于视频来说新session以为这开始视频session。 否则加入已经存在的视频session</t>
-  </si>
-  <si>
-    <t>这个存在cache中， 离开会议时使用</t>
   </si>
   <si>
     <t>0 - 无措                   40011 - 群组名字不对 50000 - 用户token不对</t>
@@ -220,14 +217,6 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -242,14 +231,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -258,7 +239,24 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -290,20 +288,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -621,86 +619,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C818839A-6A96-4C10-B0C0-B10C9919B391}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="42.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="20.140625" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -711,70 +709,70 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -785,88 +783,88 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -877,99 +875,99 @@
       <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="6"/>
+      <c r="D24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="10" t="s">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,47 +979,24 @@
       <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new JS files and updated a few
</commit_message>
<xml_diff>
--- a/MS-DB/DB api manual.xlsx
+++ b/MS-DB/DB api manual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\MS-DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48224A2E-A19F-4C04-904B-C3DC62F15CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73DD9B-CB92-457D-ACA1-0956F59DBC69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7107093B-2C12-4176-8665-F241E905E88A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -193,6 +193,42 @@
   </si>
   <si>
     <t>Session id 是一个CHAR(40)的字符串。 前端用它来控制自己的群会话。</t>
+  </si>
+  <si>
+    <t>sys_sec_group_owner_approve_user_membership_MS</t>
+  </si>
+  <si>
+    <t>@groupOwnerUsertToken</t>
+  </si>
+  <si>
+    <t>群主Token</t>
+  </si>
+  <si>
+    <t>申请用户Token</t>
+  </si>
+  <si>
+    <t>@applicationUsertToken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Parameter 3</t>
+  </si>
+  <si>
+    <t>群名字</t>
+  </si>
+  <si>
+    <t>群主批准用户入群</t>
+  </si>
+  <si>
+    <t>app_group_user_apply_for_member_MS</t>
+  </si>
+  <si>
+    <t>用户申请入群</t>
+  </si>
+  <si>
+    <t>用户·Token</t>
+  </si>
+  <si>
+    <t>界面上显示可以加入的群·名 （临时）： Fight For Trump</t>
   </si>
 </sst>
 </file>
@@ -617,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C818839A-6A96-4C10-B0C0-B10C9919B391}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66" customWidth="1"/>
+    <col min="1" max="1" width="71" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="25" style="5" customWidth="1"/>
@@ -993,10 +1029,115 @@
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>